<commit_message>
correct removal of Colonial dates
</commit_message>
<xml_diff>
--- a/SingoutInfo.xlsx
+++ b/SingoutInfo.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="231">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -68,34 +68,34 @@
     <t xml:space="preserve">black shirt, blue tie</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;&lt;Open&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapter Dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panda Inn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- none -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chehalis West</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vintage At Chehalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharon Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestige Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centralia Point</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colonial Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;&lt;Open&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapter Dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panda Inn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- none -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chehalis West</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vintage At Chehalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sharon Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prestige Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centralia Point</t>
   </si>
   <si>
     <t xml:space="preserve">polos</t>
@@ -1037,7 +1037,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.52"/>
@@ -2145,11 +2145,11 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.35"/>
@@ -2204,11 +2204,9 @@
       <c r="I2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>45309</v>
@@ -2227,10 +2225,10 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>45316</v>
@@ -2242,17 +2240,17 @@
         <v>0.8125</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>45323</v>
@@ -2271,10 +2269,10 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>45337</v>
@@ -2293,10 +2291,10 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>45358</v>
@@ -2315,10 +2313,10 @@
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>45372</v>
@@ -2337,10 +2335,10 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>45386</v>
@@ -2359,10 +2357,10 @@
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C10" s="9" t="n">
         <v>45400</v>
@@ -2425,10 +2423,10 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9" t="n">
         <v>45449</v>
@@ -2447,10 +2445,10 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>45463</v>
@@ -2469,10 +2467,10 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>45484</v>
@@ -2492,7 +2490,7 @@
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>45491</v>
@@ -2511,10 +2509,10 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>45505</v>
@@ -2662,7 +2660,7 @@
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>45554</v>
@@ -2680,11 +2678,9 @@
       <c r="I24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>45568</v>
@@ -2725,10 +2721,10 @@
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="9" t="n">
         <v>45603</v>
@@ -2747,10 +2743,10 @@
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="9" t="n">
         <v>45617</v>
@@ -2770,7 +2766,7 @@
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="9" t="n">
         <v>45631</v>
@@ -2789,10 +2785,10 @@
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="9" t="n">
         <v>45638</v>
@@ -2811,10 +2807,10 @@
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C31" s="9" t="n">
         <v>45645</v>
@@ -2923,7 +2919,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.89"/>
@@ -2950,7 +2946,7 @@
         <v>45323</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +2962,7 @@
         <v>45358</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2982,7 +2978,7 @@
         <v>45386</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,7 +3010,7 @@
         <v>45449</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,7 +3026,7 @@
         <v>45484</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3044,7 +3040,7 @@
         <v>45505</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,7 +3118,7 @@
         <v>45603</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,7 +3126,7 @@
         <v>45617</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,7 +3272,7 @@
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>61</v>
@@ -3298,7 +3294,7 @@
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>65</v>
@@ -3322,7 +3318,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>69</v>
@@ -3782,7 +3778,7 @@
     </row>
     <row r="54" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>163</v>
@@ -3816,7 +3812,7 @@
     </row>
     <row r="57" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>134</v>
@@ -3851,7 +3847,7 @@
     </row>
     <row r="60" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>174</v>
@@ -4025,7 +4021,7 @@
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>203</v>
@@ -4097,7 +4093,7 @@
     </row>
     <row r="82" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4131,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -4143,7 +4139,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4211,7 +4207,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
   </cols>
@@ -4315,7 +4311,7 @@
         <v>226</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="24" t="n">
         <v>44945</v>
@@ -4358,10 +4354,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="24" t="n">
         <v>44973</v>
@@ -4404,10 +4400,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="24" t="n">
         <v>44999</v>
@@ -4430,7 +4426,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="24" t="n">
         <v>45001</v>
@@ -4450,10 +4446,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="24" t="n">
         <v>45015</v>
@@ -4499,7 +4495,7 @@
         <v>226</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="24" t="n">
         <v>45036</v>
@@ -4519,10 +4515,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="24" t="n">
         <v>45050</v>
@@ -4565,7 +4561,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="24" t="n">
         <v>45078</v>
@@ -4577,10 +4573,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="24" t="n">
         <v>45092</v>
@@ -4600,7 +4596,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="24" t="n">
         <v>45106</v>
@@ -4615,7 +4611,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="24" t="n">
         <v>45113</v>
@@ -4635,10 +4631,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="24" t="n">
         <v>45127</v>
@@ -4797,10 +4793,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="24" t="n">
         <v>45176</v>
@@ -4820,7 +4816,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="24" t="n">
         <v>45190</v>
@@ -4855,10 +4851,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="24" t="n">
         <v>45218</v>
@@ -4881,7 +4877,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="24" t="n">
         <v>45232</v>
@@ -4904,7 +4900,7 @@
         <v>226</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="24" t="n">
         <v>45246</v>
@@ -4947,10 +4943,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="24" t="n">
         <v>45267</v>
@@ -4970,10 +4966,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" s="24" t="n">
         <v>45274</v>
@@ -4993,7 +4989,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="24" t="n">
         <v>45281</v>
@@ -13107,7 +13103,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>9</v>
@@ -13130,7 +13126,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>9</v>
@@ -13153,7 +13149,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>224</v>
@@ -13176,7 +13172,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="30" t="s">
         <v>9</v>
@@ -13199,7 +13195,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="30" t="s">
         <v>9</v>
@@ -13222,7 +13218,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>9</v>
@@ -13245,7 +13241,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="30" t="s">
         <v>9</v>
@@ -13268,7 +13264,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>9</v>
@@ -13291,7 +13287,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="30" t="s">
         <v>9</v>
@@ -13314,7 +13310,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>9</v>
@@ -13337,7 +13333,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="30" t="s">
         <v>9</v>
@@ -13360,7 +13356,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>9</v>
@@ -13383,7 +13379,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="30" t="s">
         <v>9</v>
@@ -13406,7 +13402,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="30" t="s">
         <v>9</v>
@@ -13429,7 +13425,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G16" s="30" t="s">
         <v>9</v>
@@ -13452,7 +13448,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>9</v>
@@ -13475,7 +13471,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F18" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>9</v>
@@ -13498,7 +13494,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>9</v>
@@ -13521,7 +13517,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>9</v>
@@ -13544,7 +13540,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>9</v>
@@ -13567,7 +13563,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>9</v>
@@ -13590,7 +13586,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G23" s="30" t="s">
         <v>9</v>
@@ -13613,7 +13609,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>9</v>
@@ -13636,7 +13632,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" s="30" t="s">
         <v>9</v>
@@ -13659,7 +13655,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="30" t="s">
         <v>9</v>
@@ -13682,7 +13678,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="30" t="s">
         <v>9</v>
@@ -13705,7 +13701,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="30" t="s">
         <v>9</v>
@@ -13728,7 +13724,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" s="30" t="s">
         <v>9</v>
@@ -13751,7 +13747,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" s="30" t="s">
         <v>9</v>
@@ -13774,7 +13770,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>9</v>
@@ -13797,7 +13793,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>9</v>
@@ -13820,7 +13816,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" s="30" t="s">
         <v>9</v>
@@ -13843,7 +13839,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="30" t="s">
         <v>9</v>
@@ -13866,7 +13862,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>9</v>
@@ -13889,7 +13885,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>9</v>
@@ -13912,7 +13908,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" s="30" t="s">
         <v>9</v>
@@ -13935,7 +13931,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G38" s="30" t="s">
         <v>9</v>
@@ -13958,7 +13954,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39" s="30" t="s">
         <v>9</v>
@@ -13981,7 +13977,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" s="30" t="s">
         <v>9</v>
@@ -14004,7 +14000,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" s="30" t="s">
         <v>9</v>
@@ -14027,7 +14023,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42" s="30" t="s">
         <v>9</v>
@@ -14050,7 +14046,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43" s="30" t="s">
         <v>9</v>
@@ -14073,7 +14069,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" s="30" t="s">
         <v>9</v>
@@ -14096,7 +14092,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>9</v>
@@ -14119,7 +14115,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46" s="30" t="s">
         <v>9</v>
@@ -14142,7 +14138,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G47" s="30" t="s">
         <v>9</v>
@@ -14165,7 +14161,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48" s="30" t="s">
         <v>9</v>
@@ -14188,7 +14184,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G49" s="30" t="s">
         <v>9</v>
@@ -14211,7 +14207,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G50" s="30" t="s">
         <v>9</v>
@@ -14234,7 +14230,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51" s="30" t="s">
         <v>9</v>
@@ -14257,7 +14253,7 @@
         <v>0.833333333333333</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G52" s="30" t="s">
         <v>9</v>

</xml_diff>